<commit_message>
Remove 'All other diseases (Residual)' action from US_ICD_113_SELECTED_CAUSES_ALL
</commit_message>
<xml_diff>
--- a/results/US_ICD_113_SELECTED_CAUSES_ALL/_all_b2.xlsx
+++ b/results/US_ICD_113_SELECTED_CAUSES_ALL/_all_b2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>Predicted</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>All other and unspecified malignant neoplasms</t>
-  </si>
-  <si>
-    <t>All other diseases (Residual)</t>
   </si>
   <si>
     <t>All other forms of chronic ischemic heart disease</t>
@@ -794,7 +791,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1090,19 +1087,19 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>0.05751406601729987</v>
+        <v>0.0242937866204002</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0.3850346411646618</v>
+        <v>0.3665156365095377</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
-        <v>0.9761700234267441</v>
+        <v>0.6139503769677961</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1110,19 +1107,19 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.0242937866204002</v>
+        <v>0.0214701499457541</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>0.3665156365095377</v>
+        <v>0.3915085062024354</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
-        <v>0.6139503769677961</v>
+        <v>0.7088951297304922</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1130,19 +1127,19 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.0214701499457541</v>
+        <v>0.02085059083312388</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>0.3915085062024354</v>
+        <v>0.3109781654573011</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
-        <v>0.7088951297304922</v>
+        <v>0.7657448670959528</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1150,19 +1147,19 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>0.02085059083312388</v>
+        <v>0.0007742354711494179</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>0.3109781654573011</v>
+        <v>0.4051328665849823</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18">
-        <v>0.7657448670959528</v>
+        <v>0.6471829684467595</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1170,19 +1167,19 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>0.0007742354711494179</v>
+        <v>0.001198570095971633</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>0.4051328665849823</v>
+        <v>0.4158713933231043</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
-        <v>0.6471829684467595</v>
+        <v>0.6416930768829068</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1190,19 +1187,19 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.001198570095971633</v>
+        <v>7.798755756498704e-07</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>0.4158713933231043</v>
+        <v>0.5111111111111111</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20">
-        <v>0.6416930768829068</v>
+        <v>0.6461411621166774</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1210,19 +1207,19 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>7.798755756498704e-07</v>
+        <v>0.002542654741212959</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0.5111111111111111</v>
+        <v>0.7277414488930545</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F21">
-        <v>0.6461411621166774</v>
+        <v>0.6422732939902881</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1230,19 +1227,19 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>0.002542654741212959</v>
+        <v>0.002623727789360186</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>0.7277414488930545</v>
+        <v>0.7409048371298863</v>
       </c>
       <c r="E22">
         <v>0.1</v>
       </c>
       <c r="F22">
-        <v>0.6422732939902881</v>
+        <v>0.6638401088533372</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1250,19 +1247,19 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>0.002623727789360186</v>
+        <v>0.0004555898671011315</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>0.7409048371298863</v>
+        <v>0.6934703473575711</v>
       </c>
       <c r="E23">
         <v>0.1</v>
       </c>
       <c r="F23">
-        <v>0.6638401088533372</v>
+        <v>0.6406410985369974</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1270,19 +1267,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>0.0004555898671011315</v>
+        <v>0.0004302106694665316</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>0.6934703473575711</v>
+        <v>0.5317348730373729</v>
       </c>
       <c r="E24">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0.6406410985369974</v>
+        <v>0.6445551347862609</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1290,19 +1287,19 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>0.0004302106694665316</v>
+        <v>0.0003221965453161599</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>0.5317348730373729</v>
+        <v>0.3391650853782608</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25">
-        <v>0.6445551347862609</v>
+        <v>0.6339361158443674</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1310,19 +1307,19 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>0.0003221965453161599</v>
+        <v>0.009304324317153044</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>0.3391650853782608</v>
+        <v>0.4267448137277774</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26">
-        <v>0.6339361158443674</v>
+        <v>0.6631904346518737</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1330,19 +1327,19 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>0.009304324317153044</v>
+        <v>2.811968438178345e-05</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>0.4267448137277774</v>
+        <v>0.4174755782023122</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27">
-        <v>0.6631904346518737</v>
+        <v>0.6449765743263959</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1350,19 +1347,19 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>2.811968438178345e-05</v>
+        <v>0.02391645583042436</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>0.4174755782023122</v>
+        <v>0.3705035923030724</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
-        <v>0.6449765743263959</v>
+        <v>0.7550098534512424</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1370,19 +1367,19 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>0.02391645583042436</v>
+        <v>0.0009910631963501867</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>0.3705035923030724</v>
+        <v>0.9986168502865737</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29">
-        <v>0.7550098534512424</v>
+        <v>0.6311658663056405</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1390,19 +1387,19 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>0.0009910631963501867</v>
+        <v>0.0004368991441502572</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>0.9986168502865737</v>
+        <v>0.3902300610116889</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30">
-        <v>0.6311658663056405</v>
+        <v>0.6244409877657017</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1410,19 +1407,19 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>0.0004368991441502572</v>
+        <v>0.0005577900644723376</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>0.3902300610116889</v>
+        <v>0.3734193059543309</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31">
-        <v>0.6244409877657017</v>
+        <v>0.6471790550537421</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1430,19 +1427,19 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>0.0005577900644723376</v>
+        <v>3.651143285313359e-05</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32">
-        <v>0.3734193059543309</v>
+        <v>0.458164032521354</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32">
-        <v>0.6471790550537421</v>
+        <v>0.6461411664518535</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1450,19 +1447,19 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>3.651143285313359e-05</v>
+        <v>0.007016203868866529</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>0.458164032521354</v>
+        <v>0.5176758952457914</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
       <c r="F33">
-        <v>0.6461411664518535</v>
+        <v>0.6825232071585093</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1470,19 +1467,19 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>0.007016203868866529</v>
+        <v>0.02444915173218885</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34">
-        <v>0.5176758952457914</v>
+        <v>0.391534134439024</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34">
-        <v>0.6825232071585093</v>
+        <v>0.7219369528073664</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1490,19 +1487,19 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>0.02444915173218885</v>
+        <v>0.002263014752779101</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>0.391534134439024</v>
+        <v>0.4623848643560846</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35">
-        <v>0.7219369528073664</v>
+        <v>0.6925924103025022</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1510,19 +1507,19 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>0.002263014752779101</v>
+        <v>0.001217075911345287</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36">
-        <v>0.4623848643560846</v>
+        <v>0.8060589065653649</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36">
-        <v>0.6925924103025022</v>
+        <v>0.6420796881750076</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1530,19 +1527,19 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>0.001217075911345287</v>
+        <v>0.01323351806053683</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>0.8060589065653649</v>
+        <v>0.4295458637469635</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37">
-        <v>0.6420796881750076</v>
+        <v>0.696967166161807</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1550,19 +1547,19 @@
         <v>42</v>
       </c>
       <c r="B38">
-        <v>0.01323351806053683</v>
+        <v>3.835080179834301e-05</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38">
-        <v>0.4295458637469635</v>
+        <v>0.6879477454698694</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38">
-        <v>0.696967166161807</v>
+        <v>0.6459183790595863</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1570,19 +1567,19 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>3.835080179834301e-05</v>
+        <v>4.845334924818031e-05</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39">
-        <v>0.6879477454698694</v>
+        <v>0.4580478392933712</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39">
-        <v>0.6459183790595863</v>
+        <v>0.645945341028882</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1590,19 +1587,19 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>4.845334924818031e-05</v>
+        <v>0.09626841152754827</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>0.4580478392933712</v>
+        <v>0.386122459574879</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40">
-        <v>0.645945341028882</v>
+        <v>0.8588405720481471</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1610,19 +1607,19 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>0.09626841152754827</v>
+        <v>0.0001246627182607049</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41">
-        <v>0.386122459574879</v>
+        <v>0.5062575884957996</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41">
-        <v>0.8588405720481471</v>
+        <v>0.6460486986735866</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1630,19 +1627,19 @@
         <v>46</v>
       </c>
       <c r="B42">
-        <v>0.0001246627182607049</v>
+        <v>0.0005511395579865278</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42">
-        <v>0.5062575884957996</v>
+        <v>0.4040744092637879</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42">
-        <v>0.6460486986735866</v>
+        <v>0.6350307355745519</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1650,19 +1647,19 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>0.0005511395579865278</v>
+        <v>0.006120687531974681</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>0.4040744092637879</v>
+        <v>0.3734396099331321</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43">
-        <v>0.6350307355745519</v>
+        <v>0.683035390988793</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1670,19 +1667,19 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>0.006120687531974681</v>
+        <v>0.0008128459720742385</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>0.3734396099331321</v>
+        <v>0.6541772572873235</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44">
-        <v>0.683035390988793</v>
+        <v>0.6464624666477269</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1690,19 +1687,19 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>0.0008128459720742385</v>
+        <v>0.00672606335614466</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>0.6541772572873235</v>
+        <v>0.3691618830951943</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45">
-        <v>0.6464624666477269</v>
+        <v>0.6952796400311496</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1710,19 +1707,19 @@
         <v>50</v>
       </c>
       <c r="B46">
-        <v>0.00672606335614466</v>
+        <v>0.01442514648003278</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46">
-        <v>0.3691618830951943</v>
+        <v>0.3397304764928996</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46">
-        <v>0.6952796400311496</v>
+        <v>0.7422382725349073</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1730,19 +1727,19 @@
         <v>51</v>
       </c>
       <c r="B47">
-        <v>0.01442514648003278</v>
+        <v>0.0003392807100489858</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>0.3397304764928996</v>
+        <v>0.3888608816503877</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47">
-        <v>0.7422382725349073</v>
+        <v>0.6473802323604491</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1750,19 +1747,19 @@
         <v>52</v>
       </c>
       <c r="B48">
-        <v>0.0003392807100489858</v>
+        <v>8.855431039899686e-05</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48">
-        <v>0.3888608816503877</v>
+        <v>0.486147349167496</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48">
-        <v>0.6473802323604491</v>
+        <v>0.6447605906785162</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1770,19 +1767,19 @@
         <v>53</v>
       </c>
       <c r="B49">
-        <v>8.855431039899686e-05</v>
+        <v>9.045338359863373e-05</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>0.486147349167496</v>
+        <v>0.5907569763576099</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
       <c r="F49">
-        <v>0.6447605906785162</v>
+        <v>0.6266417417227359</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1790,19 +1787,19 @@
         <v>54</v>
       </c>
       <c r="B50">
-        <v>9.045338359863373e-05</v>
+        <v>0.0001040538195983822</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50">
-        <v>0.5907569763576099</v>
+        <v>0.3251784635955832</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50">
-        <v>0.6266417417227359</v>
+        <v>0.6466423246292775</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1810,19 +1807,19 @@
         <v>55</v>
       </c>
       <c r="B51">
-        <v>0.0001040538195983822</v>
+        <v>0.002319672990287107</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>0.3251784635955832</v>
+        <v>0.3696179455263318</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51">
-        <v>0.6466423246292775</v>
+        <v>0.684204073541863</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1830,19 +1827,19 @@
         <v>56</v>
       </c>
       <c r="B52">
-        <v>0.002319672990287107</v>
+        <v>0.0103153229740922</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52">
-        <v>0.3696179455263318</v>
+        <v>0.4186468832810623</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52">
-        <v>0.684204073541863</v>
+        <v>0.7530580938423324</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1850,19 +1847,19 @@
         <v>57</v>
       </c>
       <c r="B53">
-        <v>0.0103153229740922</v>
+        <v>0.002247616674910336</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>0.4186468832810623</v>
+        <v>0.396139086741964</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53">
-        <v>0.7530580938423324</v>
+        <v>0.6479573098679596</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1870,19 +1867,19 @@
         <v>58</v>
       </c>
       <c r="B54">
-        <v>0.002247616674910336</v>
+        <v>0.0001468182816885847</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54">
-        <v>0.396139086741964</v>
+        <v>0.4191612325914973</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54">
-        <v>0.6479573098679596</v>
+        <v>0.6471492044891074</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1890,19 +1887,19 @@
         <v>59</v>
       </c>
       <c r="B55">
-        <v>0.0001468182816885847</v>
+        <v>1.856800215667738e-05</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>0.4191612325914973</v>
+        <v>0.4503100385453326</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="F55">
-        <v>0.6471492044891074</v>
+        <v>0.6461429012152158</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1910,19 +1907,19 @@
         <v>60</v>
       </c>
       <c r="B56">
-        <v>1.856800215667738e-05</v>
+        <v>0.0013764068080444</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56">
-        <v>0.4503100385453326</v>
+        <v>0.4138010929905344</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56">
-        <v>0.6461429012152158</v>
+        <v>0.6662540465816523</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1930,19 +1927,19 @@
         <v>61</v>
       </c>
       <c r="B57">
-        <v>0.0013764068080444</v>
+        <v>0.006917239028260868</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>0.4138010929905344</v>
+        <v>0.3755428444936931</v>
       </c>
       <c r="E57">
         <v>1</v>
       </c>
       <c r="F57">
-        <v>0.6662540465816523</v>
+        <v>0.6302610805538</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1950,19 +1947,19 @@
         <v>62</v>
       </c>
       <c r="B58">
-        <v>0.006917239028260868</v>
+        <v>0.00794619784491879</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58">
-        <v>0.3755428444936931</v>
+        <v>0.6265541037193831</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="F58">
-        <v>0.6302610805538</v>
+        <v>0.6880195946601132</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1970,19 +1967,19 @@
         <v>63</v>
       </c>
       <c r="B59">
-        <v>0.00794619784491879</v>
+        <v>0.004084360471415075</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59">
-        <v>0.6265541037193831</v>
+        <v>0.6022127036548905</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59">
-        <v>0.6880195946601132</v>
+        <v>0.6694914324712844</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1990,19 +1987,19 @@
         <v>64</v>
       </c>
       <c r="B60">
-        <v>0.004084360471415075</v>
+        <v>0.00385365681962658</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60">
-        <v>0.6022127036548905</v>
+        <v>0.6513471851869264</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="F60">
-        <v>0.6694914324712844</v>
+        <v>0.6648345802077089</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2010,19 +2007,19 @@
         <v>65</v>
       </c>
       <c r="B61">
-        <v>0.00385365681962658</v>
+        <v>0.04688778873600922</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>0.6513471851869264</v>
+        <v>0.3891700077462829</v>
       </c>
       <c r="E61">
         <v>1</v>
       </c>
       <c r="F61">
-        <v>0.6648345802077089</v>
+        <v>0.5589427318910586</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2030,19 +2027,19 @@
         <v>66</v>
       </c>
       <c r="B62">
-        <v>0.04688778873600922</v>
+        <v>8.647527462024655e-05</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62">
-        <v>0.3891700077462829</v>
+        <v>0.7026339376066153</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F62">
-        <v>0.5589427318910586</v>
+        <v>0.6462933446802667</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2050,19 +2047,19 @@
         <v>67</v>
       </c>
       <c r="B63">
-        <v>8.647527462024655e-05</v>
+        <v>0.003197707189119576</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>0.7026339376066153</v>
+        <v>0.4303057766341699</v>
       </c>
       <c r="E63">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F63">
-        <v>0.6462933446802667</v>
+        <v>0.6461411664518535</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2070,19 +2067,19 @@
         <v>68</v>
       </c>
       <c r="B64">
-        <v>0.003197707189119576</v>
+        <v>0.1296079354519796</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>0.4303057766341699</v>
+        <v>0.3829917413830828</v>
       </c>
       <c r="E64">
         <v>1</v>
       </c>
       <c r="F64">
-        <v>0.6461411664518535</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2090,19 +2087,19 @@
         <v>69</v>
       </c>
       <c r="B65">
-        <v>0.1296079354519796</v>
+        <v>1.114867471263882e-06</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>0.3829917413830828</v>
+        <v>0.5698757763975155</v>
       </c>
       <c r="E65">
         <v>1</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>0.6461412644225889</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2110,19 +2107,19 @@
         <v>70</v>
       </c>
       <c r="B66">
-        <v>1.114867471263882e-06</v>
+        <v>0.0007255219849146984</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66">
-        <v>0.5698757763975155</v>
+        <v>0.4485503977444972</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="F66">
-        <v>0.6461412644225889</v>
+        <v>0.6355708122529646</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2130,19 +2127,19 @@
         <v>71</v>
       </c>
       <c r="B67">
-        <v>0.0007255219849146984</v>
+        <v>0.002509705623384979</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67">
-        <v>0.4485503977444972</v>
+        <v>0.3855747008077618</v>
       </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67">
-        <v>0.6355708122529646</v>
+        <v>0.6523812225252401</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2150,19 +2147,19 @@
         <v>72</v>
       </c>
       <c r="B68">
-        <v>0.002509705623384979</v>
+        <v>0.005779680469630242</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
       <c r="D68">
-        <v>0.3855747008077618</v>
+        <v>0.454500396660768</v>
       </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68">
-        <v>0.6523812225252401</v>
+        <v>0.645384117180553</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2170,19 +2167,19 @@
         <v>73</v>
       </c>
       <c r="B69">
-        <v>0.005779680469630242</v>
+        <v>0.0005585605827767868</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>0.454500396660768</v>
+        <v>0.5322527865834952</v>
       </c>
       <c r="E69">
         <v>1</v>
       </c>
       <c r="F69">
-        <v>0.645384117180553</v>
+        <v>0.6456428181617577</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2190,19 +2187,19 @@
         <v>74</v>
       </c>
       <c r="B70">
-        <v>0.0005585605827767868</v>
+        <v>0.002197542155064421</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>0.5322527865834952</v>
+        <v>0.4494621072212744</v>
       </c>
       <c r="E70">
         <v>1</v>
       </c>
       <c r="F70">
-        <v>0.6456428181617577</v>
+        <v>0.6483782471221773</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2210,19 +2207,19 @@
         <v>75</v>
       </c>
       <c r="B71">
-        <v>0.002197542155064421</v>
+        <v>0.0004669604174727446</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71">
-        <v>0.4494621072212744</v>
+        <v>0.451839444040208</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
       <c r="F71">
-        <v>0.6483782471221773</v>
+        <v>0.6448487727129593</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2230,19 +2227,19 @@
         <v>76</v>
       </c>
       <c r="B72">
-        <v>0.0004669604174727446</v>
+        <v>0.001760728403652007</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72">
-        <v>0.451839444040208</v>
+        <v>0.4455593337791995</v>
       </c>
       <c r="E72">
         <v>1</v>
       </c>
       <c r="F72">
-        <v>0.6448487727129593</v>
+        <v>0.6411025136845979</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2250,19 +2247,19 @@
         <v>77</v>
       </c>
       <c r="B73">
-        <v>0.001760728403652007</v>
+        <v>0.007175127026483571</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73">
-        <v>0.4455593337791995</v>
+        <v>0.4300530992380643</v>
       </c>
       <c r="E73">
         <v>1</v>
       </c>
       <c r="F73">
-        <v>0.6411025136845979</v>
+        <v>0.6787778700218501</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2270,19 +2267,19 @@
         <v>78</v>
       </c>
       <c r="B74">
-        <v>0.007175127026483571</v>
+        <v>0.004771946417267393</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74">
-        <v>0.4300530992380643</v>
+        <v>0.3762511633889376</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
       <c r="F74">
-        <v>0.6787778700218501</v>
+        <v>0.6623062284971831</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2290,19 +2287,19 @@
         <v>79</v>
       </c>
       <c r="B75">
-        <v>0.004771946417267393</v>
+        <v>0.001391982992308588</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>0.3762511633889376</v>
+        <v>0.4448616906586744</v>
       </c>
       <c r="E75">
         <v>1</v>
       </c>
       <c r="F75">
-        <v>0.6623062284971831</v>
+        <v>0.6419592614959071</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2310,19 +2307,19 @@
         <v>80</v>
       </c>
       <c r="B76">
-        <v>0.001391982992308588</v>
+        <v>0.07925511379542123</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76">
-        <v>0.4448616906586744</v>
+        <v>0.4347945341765005</v>
       </c>
       <c r="E76">
         <v>1</v>
       </c>
       <c r="F76">
-        <v>0.6419592614959071</v>
+        <v>0.5648645972250034</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2330,19 +2327,19 @@
         <v>81</v>
       </c>
       <c r="B77">
-        <v>0.07925511379542123</v>
+        <v>0.006929029965173858</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77">
-        <v>0.4347945341765005</v>
+        <v>0.4341633761477224</v>
       </c>
       <c r="E77">
         <v>1</v>
       </c>
       <c r="F77">
-        <v>0.5648645972250034</v>
+        <v>0.6353771903593318</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2350,19 +2347,19 @@
         <v>82</v>
       </c>
       <c r="B78">
-        <v>0.006929029965173858</v>
+        <v>0.002012692489739575</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78">
-        <v>0.4341633761477224</v>
+        <v>0.4445199901806119</v>
       </c>
       <c r="E78">
         <v>1</v>
       </c>
       <c r="F78">
-        <v>0.6353771903593318</v>
+        <v>0.6602003130289085</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2370,19 +2367,19 @@
         <v>83</v>
       </c>
       <c r="B79">
-        <v>0.002012692489739575</v>
+        <v>0.001939798148276084</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79">
-        <v>0.4445199901806119</v>
+        <v>0.4376826615732058</v>
       </c>
       <c r="E79">
         <v>1</v>
       </c>
       <c r="F79">
-        <v>0.6602003130289085</v>
+        <v>0.6459251771811033</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2390,19 +2387,19 @@
         <v>84</v>
       </c>
       <c r="B80">
-        <v>0.001939798148276084</v>
+        <v>0.00169912670169271</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80">
-        <v>0.4376826615732058</v>
+        <v>0.4571912008538425</v>
       </c>
       <c r="E80">
         <v>1</v>
       </c>
       <c r="F80">
-        <v>0.6459251771811033</v>
+        <v>0.6544285905923308</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2410,19 +2407,19 @@
         <v>85</v>
       </c>
       <c r="B81">
-        <v>0.00169912670169271</v>
+        <v>0.00441709905342018</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81">
-        <v>0.4571912008538425</v>
+        <v>0.4575958139562537</v>
       </c>
       <c r="E81">
         <v>1</v>
       </c>
       <c r="F81">
-        <v>0.6544285905923308</v>
+        <v>0.6656875147443042</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2430,19 +2427,19 @@
         <v>86</v>
       </c>
       <c r="B82">
-        <v>0.00441709905342018</v>
+        <v>0.007664277854031783</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82">
-        <v>0.4575958139562537</v>
+        <v>0.421800007578216</v>
       </c>
       <c r="E82">
         <v>1</v>
       </c>
       <c r="F82">
-        <v>0.6656875147443042</v>
+        <v>0.6399440874921531</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2450,19 +2447,19 @@
         <v>87</v>
       </c>
       <c r="B83">
-        <v>0.007664277854031783</v>
+        <v>0.002634120164851332</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
       <c r="D83">
-        <v>0.421800007578216</v>
+        <v>0.4983263645113855</v>
       </c>
       <c r="E83">
         <v>1</v>
       </c>
       <c r="F83">
-        <v>0.6399440874921531</v>
+        <v>0.6547134047365161</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2470,19 +2467,19 @@
         <v>88</v>
       </c>
       <c r="B84">
-        <v>0.002634120164851332</v>
+        <v>0.01431945073803784</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
       <c r="D84">
-        <v>0.4983263645113855</v>
+        <v>0.4324323226504238</v>
       </c>
       <c r="E84">
         <v>1</v>
       </c>
       <c r="F84">
-        <v>0.6547134047365161</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2490,19 +2487,19 @@
         <v>89</v>
       </c>
       <c r="B85">
-        <v>0.01431945073803784</v>
+        <v>0.002871911490882582</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
       <c r="D85">
-        <v>0.4324323226504238</v>
+        <v>0.3507212316807891</v>
       </c>
       <c r="E85">
         <v>1</v>
       </c>
       <c r="F85">
-        <v>0.5</v>
+        <v>0.6979705640931249</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2510,19 +2507,16 @@
         <v>90</v>
       </c>
       <c r="B86">
-        <v>0.002871911490882582</v>
+        <v>2.835645637974225e-07</v>
       </c>
       <c r="C86">
         <v>1</v>
       </c>
-      <c r="D86">
-        <v>0.3507212316807891</v>
-      </c>
       <c r="E86">
         <v>1</v>
       </c>
       <c r="F86">
-        <v>0.6979705640931249</v>
+        <v>0.6461411664518535</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2530,16 +2524,19 @@
         <v>91</v>
       </c>
       <c r="B87">
-        <v>2.835645637974225e-07</v>
+        <v>8.409875247542502e-05</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
+      <c r="D87">
+        <v>0.5814594642641939</v>
+      </c>
       <c r="E87">
         <v>1</v>
       </c>
       <c r="F87">
-        <v>0.6461411664518535</v>
+        <v>0.6461719736437201</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2547,19 +2544,19 @@
         <v>92</v>
       </c>
       <c r="B88">
-        <v>8.409875247542502e-05</v>
+        <v>0</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88">
-        <v>0.5814594642641939</v>
+        <v>0.7046073472770397</v>
       </c>
       <c r="E88">
         <v>1</v>
       </c>
       <c r="F88">
-        <v>0.6461719736437201</v>
+        <v>0.6457549328613575</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2567,19 +2564,19 @@
         <v>93</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>0.01044912395043513</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89">
-        <v>0.7046073472770397</v>
+        <v>0.6472305324492105</v>
       </c>
       <c r="E89">
         <v>1</v>
       </c>
       <c r="F89">
-        <v>0.6457549328613575</v>
+        <v>0.6461411664518535</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2587,19 +2584,19 @@
         <v>94</v>
       </c>
       <c r="B90">
-        <v>0.01044912395043513</v>
+        <v>0.00181038956134994</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90">
-        <v>0.6472305324492105</v>
+        <v>0.4128774496482169</v>
       </c>
       <c r="E90">
         <v>1</v>
       </c>
       <c r="F90">
-        <v>0.6461411664518535</v>
+        <v>0.647707845499495</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2607,19 +2604,19 @@
         <v>95</v>
       </c>
       <c r="B91">
-        <v>0.00181038956134994</v>
+        <v>0.00771803921248306</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91">
-        <v>0.4128774496482169</v>
+        <v>0.3876199639735308</v>
       </c>
       <c r="E91">
         <v>1</v>
       </c>
       <c r="F91">
-        <v>0.647707845499495</v>
+        <v>0.6683788133204051</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2627,19 +2624,19 @@
         <v>96</v>
       </c>
       <c r="B92">
-        <v>0.00771803921248306</v>
+        <v>0.002747604910281996</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92">
-        <v>0.3876199639735308</v>
+        <v>0.4142618205490511</v>
       </c>
       <c r="E92">
         <v>1</v>
       </c>
       <c r="F92">
-        <v>0.6683788133204051</v>
+        <v>0.6448952980638915</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2647,19 +2644,19 @@
         <v>97</v>
       </c>
       <c r="B93">
-        <v>0.002747604910281996</v>
+        <v>0.02809905270139234</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="D93">
-        <v>0.4142618205490511</v>
+        <v>0.5418954524108834</v>
       </c>
       <c r="E93">
         <v>1</v>
       </c>
       <c r="F93">
-        <v>0.6448952980638915</v>
+        <v>0.9453037788065672</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2667,19 +2664,19 @@
         <v>98</v>
       </c>
       <c r="B94">
-        <v>0.02809905270139234</v>
+        <v>0.002947647653539877</v>
       </c>
       <c r="C94">
         <v>1</v>
       </c>
       <c r="D94">
-        <v>0.5418954524108834</v>
+        <v>0.3516697815129814</v>
       </c>
       <c r="E94">
         <v>1</v>
       </c>
       <c r="F94">
-        <v>0.9453037788065672</v>
+        <v>0.6991506084904239</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2687,19 +2684,19 @@
         <v>99</v>
       </c>
       <c r="B95">
-        <v>0.002947647653539877</v>
+        <v>0</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
       <c r="D95">
-        <v>0.3516697815129814</v>
+        <v>0.4545332257196665</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F95">
-        <v>0.6991506084904239</v>
+        <v>0.6460892193564305</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2707,19 +2704,19 @@
         <v>100</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>0.0006291527123589937</v>
       </c>
       <c r="C96">
         <v>1</v>
       </c>
       <c r="D96">
-        <v>0.4545332257196665</v>
+        <v>0.4064390138171681</v>
       </c>
       <c r="E96">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F96">
-        <v>0.6460892193564305</v>
+        <v>0.6467185511584347</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2727,19 +2724,19 @@
         <v>101</v>
       </c>
       <c r="B97">
-        <v>0.0006291527123589937</v>
+        <v>2.690800557970337e-05</v>
       </c>
       <c r="C97">
         <v>1</v>
       </c>
       <c r="D97">
-        <v>0.4064390138171681</v>
+        <v>0.5055606954079255</v>
       </c>
       <c r="E97">
         <v>1</v>
       </c>
       <c r="F97">
-        <v>0.6467185511584347</v>
+        <v>0.6457748926559375</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2747,19 +2744,19 @@
         <v>102</v>
       </c>
       <c r="B98">
-        <v>2.690800557970337e-05</v>
+        <v>1.069407671257506e-05</v>
       </c>
       <c r="C98">
         <v>1</v>
       </c>
       <c r="D98">
-        <v>0.5055606954079255</v>
+        <v>0.3878021675419445</v>
       </c>
       <c r="E98">
         <v>1</v>
       </c>
       <c r="F98">
-        <v>0.6457748926559375</v>
+        <v>0.6461972016717082</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2767,19 +2764,19 @@
         <v>103</v>
       </c>
       <c r="B99">
-        <v>1.069407671257506e-05</v>
+        <v>0.0007875670051052837</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
       <c r="D99">
-        <v>0.3878021675419445</v>
+        <v>0.652134648190269</v>
       </c>
       <c r="E99">
         <v>1</v>
       </c>
       <c r="F99">
-        <v>0.6461972016717082</v>
+        <v>0.647053939141476</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2787,19 +2784,19 @@
         <v>104</v>
       </c>
       <c r="B100">
-        <v>0.0007875670051052837</v>
+        <v>0.001152370796841572</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
       <c r="D100">
-        <v>0.652134648190269</v>
+        <v>0.4616943540423675</v>
       </c>
       <c r="E100">
         <v>1</v>
       </c>
       <c r="F100">
-        <v>0.647053939141476</v>
+        <v>0.6497746318582309</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2807,19 +2804,19 @@
         <v>105</v>
       </c>
       <c r="B101">
-        <v>0.001152370796841572</v>
+        <v>1.711989229018788e-05</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101">
-        <v>0.4616943540423675</v>
+        <v>0.4163509131251066</v>
       </c>
       <c r="E101">
         <v>1</v>
       </c>
       <c r="F101">
-        <v>0.6497746318582309</v>
+        <v>0.6462344520699144</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2827,19 +2824,19 @@
         <v>106</v>
       </c>
       <c r="B102">
-        <v>1.711989229018788e-05</v>
+        <v>0.002356680068697614</v>
       </c>
       <c r="C102">
         <v>1</v>
       </c>
       <c r="D102">
-        <v>0.4163509131251066</v>
+        <v>0.4911085498974804</v>
       </c>
       <c r="E102">
         <v>1</v>
       </c>
       <c r="F102">
-        <v>0.6462344520699144</v>
+        <v>0.6401941194855698</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2847,19 +2844,19 @@
         <v>107</v>
       </c>
       <c r="B103">
-        <v>0.002356680068697614</v>
+        <v>0.003006026734760968</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
       <c r="D103">
-        <v>0.4911085498974804</v>
+        <v>0.4812546489677728</v>
       </c>
       <c r="E103">
         <v>1</v>
       </c>
       <c r="F103">
-        <v>0.6401941194855698</v>
+        <v>0.6555778973913252</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2867,19 +2864,19 @@
         <v>108</v>
       </c>
       <c r="B104">
-        <v>0.003006026734760968</v>
+        <v>0.02232132600529926</v>
       </c>
       <c r="C104">
         <v>1</v>
       </c>
       <c r="D104">
-        <v>0.4812546489677728</v>
+        <v>0.3872078866224863</v>
       </c>
       <c r="E104">
         <v>1</v>
       </c>
       <c r="F104">
-        <v>0.6555778973913252</v>
+        <v>0.6999794631391374</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2887,19 +2884,19 @@
         <v>109</v>
       </c>
       <c r="B105">
-        <v>0.02232132600529926</v>
+        <v>0.0002148469651257631</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
       <c r="D105">
-        <v>0.3872078866224863</v>
+        <v>0.723228608426034</v>
       </c>
       <c r="E105">
         <v>1</v>
       </c>
       <c r="F105">
-        <v>0.6999794631391374</v>
+        <v>0.6475383259552059</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2907,19 +2904,19 @@
         <v>110</v>
       </c>
       <c r="B106">
-        <v>0.0002148469651257631</v>
+        <v>0.001396610077216232</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
       <c r="D106">
-        <v>0.723228608426034</v>
+        <v>0.3837602549539634</v>
       </c>
       <c r="E106">
         <v>1</v>
       </c>
       <c r="F106">
-        <v>0.6475383259552059</v>
+        <v>0.6474793298739836</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2927,19 +2924,19 @@
         <v>111</v>
       </c>
       <c r="B107">
-        <v>0.001396610077216232</v>
+        <v>0.002695334074978345</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107">
-        <v>0.3837602549539634</v>
+        <v>0.4001308852912836</v>
       </c>
       <c r="E107">
         <v>1</v>
       </c>
       <c r="F107">
-        <v>0.6474793298739836</v>
+        <v>0.6459909619772607</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2947,19 +2944,19 @@
         <v>112</v>
       </c>
       <c r="B108">
-        <v>0.002695334074978345</v>
+        <v>0.007262722426271506</v>
       </c>
       <c r="C108">
         <v>1</v>
       </c>
       <c r="D108">
-        <v>0.4001308852912836</v>
+        <v>0.4025806330982485</v>
       </c>
       <c r="E108">
         <v>1</v>
       </c>
       <c r="F108">
-        <v>0.6459909619772607</v>
+        <v>0.6906796295008453</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2967,19 +2964,19 @@
         <v>113</v>
       </c>
       <c r="B109">
-        <v>0.007262722426271506</v>
+        <v>0.0006190644292282908</v>
       </c>
       <c r="C109">
         <v>1</v>
       </c>
       <c r="D109">
-        <v>0.4025806330982485</v>
+        <v>0.4728036399288283</v>
       </c>
       <c r="E109">
         <v>1</v>
       </c>
       <c r="F109">
-        <v>0.6906796295008453</v>
+        <v>0.6452479426606418</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2987,19 +2984,19 @@
         <v>114</v>
       </c>
       <c r="B110">
-        <v>0.0006190644292282908</v>
+        <v>2.508798267187842e-06</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
       <c r="D110">
-        <v>0.4728036399288283</v>
+        <v>0.4546957671957672</v>
       </c>
       <c r="E110">
         <v>1</v>
       </c>
       <c r="F110">
-        <v>0.6452479426606418</v>
+        <v>0.6461248380044737</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3007,19 +3004,19 @@
         <v>115</v>
       </c>
       <c r="B111">
-        <v>2.508798267187842e-06</v>
+        <v>0.03361809612875008</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111">
-        <v>0.4546957671957672</v>
+        <v>0.3813852085776138</v>
       </c>
       <c r="E111">
         <v>1</v>
       </c>
       <c r="F111">
-        <v>0.6461248380044737</v>
+        <v>0.6300419232983669</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3027,19 +3024,19 @@
         <v>116</v>
       </c>
       <c r="B112">
-        <v>0.03361809612875008</v>
+        <v>0.03623962950256651</v>
       </c>
       <c r="C112">
         <v>1</v>
       </c>
       <c r="D112">
-        <v>0.3813852085776138</v>
+        <v>0.374739738130443</v>
       </c>
       <c r="E112">
         <v>1</v>
       </c>
       <c r="F112">
-        <v>0.6300419232983669</v>
+        <v>0.8051532967837178</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3047,19 +3044,19 @@
         <v>117</v>
       </c>
       <c r="B113">
-        <v>0.03623962950256651</v>
+        <v>6.652051800075898e-05</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
       <c r="D113">
-        <v>0.374739738130443</v>
+        <v>0.6326920147457575</v>
       </c>
       <c r="E113">
         <v>1</v>
       </c>
       <c r="F113">
-        <v>0.8051532967837178</v>
+        <v>0.6438014724590991</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3067,19 +3064,19 @@
         <v>118</v>
       </c>
       <c r="B114">
-        <v>6.652051800075898e-05</v>
+        <v>3.281829006860156e-05</v>
       </c>
       <c r="C114">
         <v>1</v>
       </c>
       <c r="D114">
-        <v>0.6326920147457575</v>
+        <v>0.3761216029086125</v>
       </c>
       <c r="E114">
         <v>1</v>
       </c>
       <c r="F114">
-        <v>0.6438014724590991</v>
+        <v>0.6461411664518535</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3087,19 +3084,19 @@
         <v>119</v>
       </c>
       <c r="B115">
-        <v>3.281829006860156e-05</v>
+        <v>1.925716815970508e-05</v>
       </c>
       <c r="C115">
         <v>1</v>
       </c>
       <c r="D115">
-        <v>0.3761216029086125</v>
+        <v>0.4698989498378825</v>
       </c>
       <c r="E115">
         <v>1</v>
       </c>
       <c r="F115">
-        <v>0.6461411664518535</v>
+        <v>0.6460418221352189</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3107,19 +3104,19 @@
         <v>120</v>
       </c>
       <c r="B116">
-        <v>1.925716815970508e-05</v>
+        <v>0.006734775117730791</v>
       </c>
       <c r="C116">
         <v>1</v>
       </c>
       <c r="D116">
-        <v>0.4698989498378825</v>
+        <v>0.3475955367919121</v>
       </c>
       <c r="E116">
         <v>1</v>
       </c>
       <c r="F116">
-        <v>0.6460418221352189</v>
+        <v>0.7133235367777053</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3127,19 +3124,19 @@
         <v>121</v>
       </c>
       <c r="B117">
-        <v>0.006734775117730791</v>
+        <v>0.0005753987829770467</v>
       </c>
       <c r="C117">
         <v>1</v>
       </c>
       <c r="D117">
-        <v>0.3475955367919121</v>
+        <v>0.4125162058037573</v>
       </c>
       <c r="E117">
         <v>1</v>
       </c>
       <c r="F117">
-        <v>0.7133235367777053</v>
+        <v>0.6495851366820834</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3147,19 +3144,19 @@
         <v>122</v>
       </c>
       <c r="B118">
-        <v>0.0005753987829770467</v>
+        <v>4.616698747892953e-05</v>
       </c>
       <c r="C118">
         <v>1</v>
       </c>
       <c r="D118">
-        <v>0.4125162058037573</v>
+        <v>0.3701981522003404</v>
       </c>
       <c r="E118">
         <v>1</v>
       </c>
       <c r="F118">
-        <v>0.6495851366820834</v>
+        <v>0.6448232807721717</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3167,19 +3164,19 @@
         <v>123</v>
       </c>
       <c r="B119">
-        <v>4.616698747892953e-05</v>
+        <v>0.005421765537489459</v>
       </c>
       <c r="C119">
         <v>1</v>
       </c>
       <c r="D119">
-        <v>0.3701981522003404</v>
+        <v>0.3720730129950783</v>
       </c>
       <c r="E119">
         <v>1</v>
       </c>
       <c r="F119">
-        <v>0.6448232807721717</v>
+        <v>0.6097654064468662</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3187,19 +3184,19 @@
         <v>124</v>
       </c>
       <c r="B120">
-        <v>0.005421765537489459</v>
+        <v>0.003033931067899758</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
       <c r="D120">
-        <v>0.3720730129950783</v>
+        <v>0.3590558922727385</v>
       </c>
       <c r="E120">
         <v>1</v>
       </c>
       <c r="F120">
-        <v>0.6097654064468662</v>
+        <v>0.6541038802087733</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3207,19 +3204,19 @@
         <v>125</v>
       </c>
       <c r="B121">
-        <v>0.003033931067899758</v>
+        <v>6.535448796314413e-07</v>
       </c>
       <c r="C121">
         <v>1</v>
       </c>
       <c r="D121">
-        <v>0.3590558922727385</v>
+        <v>0.7541735084838533</v>
       </c>
       <c r="E121">
         <v>1</v>
       </c>
       <c r="F121">
-        <v>0.6541038802087733</v>
+        <v>0.6460837763768404</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -3227,19 +3224,19 @@
         <v>126</v>
       </c>
       <c r="B122">
-        <v>6.535448796314413e-07</v>
+        <v>0.0002150173933102162</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
       <c r="D122">
-        <v>0.7541735084838533</v>
+        <v>0.7238406473700592</v>
       </c>
       <c r="E122">
         <v>1</v>
       </c>
       <c r="F122">
-        <v>0.6460837763768404</v>
+        <v>0.6474697590549967</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3247,19 +3244,19 @@
         <v>127</v>
       </c>
       <c r="B123">
-        <v>0.0002150173933102162</v>
+        <v>0.007157099929557553</v>
       </c>
       <c r="C123">
         <v>1</v>
       </c>
       <c r="D123">
-        <v>0.7238406473700592</v>
+        <v>0.3871946207171476</v>
       </c>
       <c r="E123">
         <v>1</v>
       </c>
       <c r="F123">
-        <v>0.6474697590549967</v>
+        <v>0.6561610261273045</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3267,19 +3264,19 @@
         <v>128</v>
       </c>
       <c r="B124">
-        <v>0.007157099929557553</v>
+        <v>2.709495364634357e-05</v>
       </c>
       <c r="C124">
         <v>1</v>
       </c>
       <c r="D124">
-        <v>0.3871946207171476</v>
+        <v>0.4405262405262405</v>
       </c>
       <c r="E124">
         <v>1</v>
       </c>
       <c r="F124">
-        <v>0.6561610261273045</v>
+        <v>0.6455392854305076</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3287,19 +3284,19 @@
         <v>129</v>
       </c>
       <c r="B125">
-        <v>2.709495364634357e-05</v>
+        <v>6.275627430796251e-06</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125">
-        <v>0.4405262405262405</v>
+        <v>0.4873710924998137</v>
       </c>
       <c r="E125">
         <v>1</v>
       </c>
       <c r="F125">
-        <v>0.6455392854305076</v>
+        <v>0.6461375436304709</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3307,19 +3304,19 @@
         <v>130</v>
       </c>
       <c r="B126">
-        <v>6.275627430796251e-06</v>
+        <v>0</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
       <c r="D126">
-        <v>0.4873710924998137</v>
+        <v>0.4809523809523809</v>
       </c>
       <c r="E126">
         <v>1</v>
       </c>
       <c r="F126">
-        <v>0.6461375436304709</v>
+        <v>0.6461265024163083</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3327,19 +3324,19 @@
         <v>131</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>0.005951263841515607</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127">
-        <v>0.4809523809523809</v>
+        <v>0.4147362207297287</v>
       </c>
       <c r="E127">
         <v>1</v>
       </c>
       <c r="F127">
-        <v>0.6461265024163083</v>
+        <v>0.6559126136355016</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3347,19 +3344,19 @@
         <v>132</v>
       </c>
       <c r="B128">
-        <v>0.005951263841515607</v>
+        <v>3.719304223254379e-07</v>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128">
-        <v>0.4147362207297287</v>
+        <v>0.5451559934318555</v>
       </c>
       <c r="E128">
         <v>1</v>
       </c>
       <c r="F128">
-        <v>0.6559126136355016</v>
+        <v>0.6461319201344609</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3367,19 +3364,19 @@
         <v>133</v>
       </c>
       <c r="B129">
-        <v>3.719304223254379e-07</v>
+        <v>0.004517301568152653</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129">
-        <v>0.5451559934318555</v>
+        <v>0.4563379683366033</v>
       </c>
       <c r="E129">
         <v>1</v>
       </c>
       <c r="F129">
-        <v>0.6461319201344609</v>
+        <v>0.6461411664518535</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3387,19 +3384,19 @@
         <v>134</v>
       </c>
       <c r="B130">
-        <v>0.004517301568152653</v>
+        <v>1.125308667723854e-05</v>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130">
-        <v>0.4563379683366033</v>
+        <v>0.4660674997348976</v>
       </c>
       <c r="E130">
         <v>1</v>
       </c>
       <c r="F130">
-        <v>0.6461411664518535</v>
+        <v>0.6462155414878057</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3407,19 +3404,19 @@
         <v>135</v>
       </c>
       <c r="B131">
-        <v>1.125308667723854e-05</v>
+        <v>0.00577574542053005</v>
       </c>
       <c r="C131">
         <v>1</v>
       </c>
       <c r="D131">
-        <v>0.4660674997348976</v>
+        <v>0.6452460530793734</v>
       </c>
       <c r="E131">
         <v>1</v>
       </c>
       <c r="F131">
-        <v>0.6462155414878057</v>
+        <v>0.6419420340514543</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3427,19 +3424,19 @@
         <v>136</v>
       </c>
       <c r="B132">
-        <v>0.00577574542053005</v>
+        <v>5.965721737958838e-05</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
       <c r="D132">
-        <v>0.6452460530793734</v>
+        <v>0.4489427168156929</v>
       </c>
       <c r="E132">
         <v>1</v>
       </c>
       <c r="F132">
-        <v>0.6419420340514543</v>
+        <v>0.645813130643726</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3447,19 +3444,19 @@
         <v>137</v>
       </c>
       <c r="B133">
-        <v>5.965721737958838e-05</v>
+        <v>0</v>
       </c>
       <c r="C133">
         <v>1</v>
       </c>
       <c r="D133">
-        <v>0.4489427168156929</v>
+        <v>0.5189715343856574</v>
       </c>
       <c r="E133">
         <v>1</v>
       </c>
       <c r="F133">
-        <v>0.645813130643726</v>
+        <v>0.6189484069298427</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3467,19 +3464,19 @@
         <v>138</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>0.0002623122422698695</v>
       </c>
       <c r="C134">
         <v>1</v>
       </c>
       <c r="D134">
-        <v>0.5189715343856574</v>
+        <v>0.6074793745344337</v>
       </c>
       <c r="E134">
         <v>1</v>
       </c>
       <c r="F134">
-        <v>0.6189484069298427</v>
+        <v>0.64699660958117</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3487,38 +3484,18 @@
         <v>139</v>
       </c>
       <c r="B135">
-        <v>0.0002623122422698695</v>
+        <v>2.414759699350312e-06</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135">
-        <v>0.6074793745344337</v>
+        <v>0.8512230696522278</v>
       </c>
       <c r="E135">
         <v>1</v>
       </c>
       <c r="F135">
-        <v>0.64699660958117</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B136">
-        <v>2.414759699350312e-06</v>
-      </c>
-      <c r="C136">
-        <v>1</v>
-      </c>
-      <c r="D136">
-        <v>0.8512230696522278</v>
-      </c>
-      <c r="E136">
-        <v>1</v>
-      </c>
-      <c r="F136">
         <v>0.6461491150114956</v>
       </c>
     </row>

</xml_diff>